<commit_message>
Updated the Names of TC
</commit_message>
<xml_diff>
--- a/ACME_Test_Demo/Data/Config.xlsx
+++ b/ACME_Test_Demo/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PRASHANT\ACCELIRATE\workspace\MySamples\ACME_Test_Demo\ACME_Test_Demo\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PRASHANT\ACCELIRATE\workspace\MySamples\github\UiPath_Repo\ACME_Test_Demo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7356FF75-AD03-46AE-9934-5C386FDB1BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059A1DB7-61C5-4EED-A636-D5699A6E0FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -832,7 +832,7 @@
         <v>72</v>
       </c>
       <c r="B21">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>